<commit_message>
🦄 refactor: use Anchor Component
</commit_message>
<xml_diff>
--- a/public/說明書_測試.xlsx
+++ b/public/說明書_測試.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="58">
   <si>
     <t>tag</t>
   </si>
@@ -165,6 +165,27 @@
   </si>
   <si>
     <t>單一功能名稱 5.2.2</t>
+  </si>
+  <si>
+    <t>頁面名稱 -6</t>
+  </si>
+  <si>
+    <t>功能區塊 6.1</t>
+  </si>
+  <si>
+    <t>單一功能名稱 6.1.1</t>
+  </si>
+  <si>
+    <t>單一功能名稱 6.1.2</t>
+  </si>
+  <si>
+    <t>功能區塊 6.2</t>
+  </si>
+  <si>
+    <t>單一功能名稱 6.2.1</t>
+  </si>
+  <si>
+    <t>單一功能名稱 6.2.2</t>
   </si>
 </sst>
 </file>
@@ -1619,204 +1640,332 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="11"/>
-      <c r="B138" s="8"/>
+      <c r="A138" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C138" s="8"/>
     </row>
     <row r="139">
-      <c r="A139" s="11"/>
-      <c r="B139" s="8"/>
+      <c r="A139" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="C139" s="8"/>
     </row>
     <row r="140">
-      <c r="A140" s="11"/>
-      <c r="B140" s="8"/>
+      <c r="A140" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="C140" s="8"/>
     </row>
     <row r="141">
-      <c r="A141" s="11"/>
-      <c r="B141" s="8"/>
+      <c r="A141" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="C141" s="8"/>
     </row>
     <row r="142">
-      <c r="A142" s="11"/>
-      <c r="B142" s="8"/>
+      <c r="A142" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C142" s="8"/>
     </row>
     <row r="143">
-      <c r="A143" s="11"/>
-      <c r="B143" s="8"/>
+      <c r="A143" s="7"/>
+      <c r="B143" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C143" s="8"/>
     </row>
     <row r="144">
-      <c r="A144" s="11"/>
-      <c r="B144" s="8"/>
+      <c r="A144" s="7"/>
+      <c r="B144" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C144" s="8"/>
     </row>
     <row r="145">
-      <c r="A145" s="11"/>
-      <c r="B145" s="8"/>
+      <c r="A145" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="C145" s="8"/>
     </row>
     <row r="146">
-      <c r="A146" s="11"/>
-      <c r="B146" s="8"/>
+      <c r="A146" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C146" s="8"/>
     </row>
     <row r="147">
-      <c r="A147" s="11"/>
-      <c r="B147" s="8"/>
+      <c r="A147" s="7"/>
+      <c r="B147" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C147" s="8"/>
     </row>
     <row r="148">
-      <c r="A148" s="11"/>
-      <c r="B148" s="8"/>
+      <c r="A148" s="7"/>
+      <c r="B148" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C148" s="8"/>
     </row>
     <row r="149">
-      <c r="A149" s="11"/>
-      <c r="B149" s="8"/>
+      <c r="A149" s="7"/>
+      <c r="B149" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C149" s="8"/>
     </row>
     <row r="150">
-      <c r="A150" s="11"/>
-      <c r="B150" s="8"/>
+      <c r="A150" s="4"/>
+      <c r="B150" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C150" s="8"/>
     </row>
     <row r="151">
-      <c r="A151" s="11"/>
-      <c r="B151" s="8"/>
-      <c r="C151" s="8"/>
+      <c r="A151" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="152">
-      <c r="A152" s="11"/>
-      <c r="B152" s="8"/>
+      <c r="A152" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="C152" s="8"/>
     </row>
     <row r="153">
-      <c r="A153" s="11"/>
-      <c r="B153" s="8"/>
+      <c r="A153" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C153" s="8"/>
     </row>
     <row r="154">
-      <c r="A154" s="11"/>
-      <c r="B154" s="8"/>
+      <c r="A154" s="7"/>
+      <c r="B154" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C154" s="8"/>
     </row>
     <row r="155">
-      <c r="A155" s="11"/>
-      <c r="B155" s="8"/>
+      <c r="A155" s="7"/>
+      <c r="B155" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C155" s="8"/>
     </row>
     <row r="156">
-      <c r="A156" s="11"/>
-      <c r="B156" s="8"/>
+      <c r="A156" s="7"/>
+      <c r="B156" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C156" s="8"/>
     </row>
     <row r="157">
-      <c r="A157" s="11"/>
-      <c r="B157" s="8"/>
+      <c r="A157" s="4"/>
+      <c r="B157" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C157" s="8"/>
     </row>
     <row r="158">
-      <c r="A158" s="11"/>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
+      <c r="A158" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="159">
-      <c r="A159" s="11"/>
-      <c r="B159" s="8"/>
+      <c r="A159" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="C159" s="8"/>
     </row>
     <row r="160">
-      <c r="A160" s="11"/>
-      <c r="B160" s="8"/>
+      <c r="A160" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="C160" s="8"/>
     </row>
     <row r="161">
-      <c r="A161" s="11"/>
-      <c r="B161" s="8"/>
+      <c r="A161" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C161" s="8"/>
     </row>
     <row r="162">
-      <c r="A162" s="11"/>
-      <c r="B162" s="8"/>
+      <c r="A162" s="7"/>
+      <c r="B162" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C162" s="8"/>
     </row>
     <row r="163">
-      <c r="A163" s="11"/>
-      <c r="B163" s="8"/>
+      <c r="A163" s="7"/>
+      <c r="B163" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C163" s="8"/>
     </row>
     <row r="164">
-      <c r="A164" s="11"/>
-      <c r="B164" s="8"/>
+      <c r="A164" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="C164" s="8"/>
     </row>
     <row r="165">
-      <c r="A165" s="11"/>
-      <c r="B165" s="8"/>
+      <c r="A165" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C165" s="8"/>
     </row>
     <row r="166">
-      <c r="A166" s="11"/>
-      <c r="B166" s="8"/>
+      <c r="A166" s="7"/>
+      <c r="B166" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C166" s="8"/>
     </row>
     <row r="167">
-      <c r="A167" s="11"/>
-      <c r="B167" s="8"/>
+      <c r="A167" s="7"/>
+      <c r="B167" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C167" s="8"/>
     </row>
     <row r="168">
-      <c r="A168" s="11"/>
-      <c r="B168" s="8"/>
+      <c r="A168" s="7"/>
+      <c r="B168" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C168" s="8"/>
     </row>
     <row r="169">
-      <c r="A169" s="11"/>
-      <c r="B169" s="8"/>
+      <c r="A169" s="4"/>
+      <c r="B169" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C169" s="8"/>
     </row>
     <row r="170">
-      <c r="A170" s="11"/>
-      <c r="B170" s="8"/>
-      <c r="C170" s="8"/>
+      <c r="A170" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="171">
-      <c r="A171" s="11"/>
-      <c r="B171" s="8"/>
+      <c r="A171" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="C171" s="8"/>
     </row>
     <row r="172">
-      <c r="A172" s="11"/>
-      <c r="B172" s="8"/>
+      <c r="A172" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C172" s="8"/>
     </row>
     <row r="173">
-      <c r="A173" s="11"/>
-      <c r="B173" s="8"/>
+      <c r="A173" s="7"/>
+      <c r="B173" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C173" s="8"/>
     </row>
     <row r="174">
-      <c r="A174" s="11"/>
-      <c r="B174" s="8"/>
+      <c r="A174" s="7"/>
+      <c r="B174" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C174" s="8"/>
     </row>
     <row r="175">
-      <c r="A175" s="11"/>
-      <c r="B175" s="8"/>
+      <c r="A175" s="7"/>
+      <c r="B175" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C175" s="8"/>
     </row>
     <row r="176">
-      <c r="A176" s="11"/>
-      <c r="B176" s="8"/>
+      <c r="A176" s="4"/>
+      <c r="B176" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C176" s="8"/>
     </row>
     <row r="177">
-      <c r="A177" s="11"/>
-      <c r="B177" s="8"/>
-      <c r="C177" s="8"/>
+      <c r="A177" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="11"/>

</xml_diff>